<commit_message>
Currently debugging an issue where the pose increments before the first pose has even been run.
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Action</t>
   </si>
@@ -64,6 +64,45 @@
   </si>
   <si>
     <t>timerUI() displays 4 seconds.</t>
+  </si>
+  <si>
+    <t>Timer Value is now 3.</t>
+  </si>
+  <si>
+    <t>timerUI() displays 3 seconds.</t>
+  </si>
+  <si>
+    <t>Timer Value is now 2.</t>
+  </si>
+  <si>
+    <t>timerUI() displays 2 seconds.</t>
+  </si>
+  <si>
+    <t>Timer Value is now 1.</t>
+  </si>
+  <si>
+    <t>timerUI() displays 1 seconds.</t>
+  </si>
+  <si>
+    <t>Timer Value is now 0.</t>
+  </si>
+  <si>
+    <t>False (because timer value is 0).</t>
+  </si>
+  <si>
+    <t>runCountdownTimer() checks if audio is on.</t>
+  </si>
+  <si>
+    <t>If true, plays audio.  If false, does not.</t>
+  </si>
+  <si>
+    <t>runCountdownTimer() checks if transition is true.</t>
+  </si>
+  <si>
+    <t>runCountdownTimer() sets transition to false.</t>
+  </si>
+  <si>
+    <t>transition is now false.</t>
   </si>
 </sst>
 </file>
@@ -128,9 +167,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,6 +550,147 @@
       </c>
       <c r="B8" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still debugging. Once transition gets set to false, breakages begin. Saving progress for the night.
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Action</t>
   </si>
@@ -93,9 +93,6 @@
     <t>runCountdownTimer() checks if audio is on.</t>
   </si>
   <si>
-    <t>If true, plays audio.  If false, does not.</t>
-  </si>
-  <si>
     <t>runCountdownTimer() checks if transition is true.</t>
   </si>
   <si>
@@ -103,6 +100,12 @@
   </si>
   <si>
     <t>transition is now false.</t>
+  </si>
+  <si>
+    <t>If true, plays "next" audio.  If false, does not.</t>
+  </si>
+  <si>
+    <t>timerUI() displays 0 seconds.</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,12 +672,12 @@
         <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
@@ -682,15 +685,18 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>